<commit_message>
changing layout for the EIAN analysis workbook
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Other_workbooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="0" windowWidth="15345" windowHeight="16905" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="25480" windowHeight="16580" tabRatio="817" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
   <si>
     <t>mouse name</t>
   </si>
@@ -187,12 +182,6 @@
     <t>pair/cell number</t>
   </si>
   <si>
-    <t>cells in pair</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>CH_070714_A</t>
   </si>
   <si>
@@ -260,6 +249,12 @@
   </si>
   <si>
     <t>Need to use histology to verify HVA</t>
+  </si>
+  <si>
+    <t>analyze cell 2</t>
+  </si>
+  <si>
+    <t>analyze cell 1</t>
   </si>
 </sst>
 </file>
@@ -329,8 +324,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -405,7 +402,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +415,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +428,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -769,24 +768,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.875" defaultRowHeight="26.1" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="75" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="33.875" style="1"/>
+    <col min="8" max="16384" width="33.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -806,7 +805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="26" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -826,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="26" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -846,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="26" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -866,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="26" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -886,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="26" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -906,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="26" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -926,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="26" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -949,7 +948,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="26" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -972,7 +971,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="26" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -995,7 +994,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1018,7 +1017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="26" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="26" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="26" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="26" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="26" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="26" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="26" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="26" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="26" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="26" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="26" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="26" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="26" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="26" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="26" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1321,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="26" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1341,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="26" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1364,7 +1363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="26" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1384,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="26" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="26" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1424,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="26" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1447,7 +1446,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="26" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="26" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="26" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="26" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="26" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1556,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="26" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="26" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="26" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="26" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1655,302 +1654,338 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="9" style="14"/>
-    <col min="5" max="5" width="11.375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="13" style="15" customWidth="1"/>
-    <col min="7" max="7" width="9" style="15"/>
-    <col min="8" max="8" width="46.5" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="13"/>
+    <col min="2" max="2" width="12.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="14"/>
+    <col min="6" max="6" width="11.33203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="13" style="15" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="15"/>
+    <col min="9" max="9" width="46.5" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>53</v>
+      <c r="C1" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="21" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="H2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="35.25" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14">
-        <v>2</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="14">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14">
-        <v>2</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14">
-        <v>2</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="14">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14" t="s">
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="F12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" s="14">
-        <v>1</v>
-      </c>
-      <c r="C11" s="14">
-        <v>2</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="14">
-        <v>1</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="B13" s="14">
         <v>3</v>
@@ -1958,68 +1993,82 @@
       <c r="C13" s="14">
         <v>1</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="F13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
       </c>
       <c r="C15" s="14">
-        <v>2</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2031,14 +2080,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.375" defaultRowHeight="26.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="20.375" style="6"/>
-    <col min="4" max="4" width="20.375" style="7"/>
-    <col min="5" max="16384" width="20.375" style="6"/>
+    <col min="1" max="3" width="20.33203125" style="6"/>
+    <col min="4" max="4" width="20.33203125" style="7"/>
+    <col min="5" max="16384" width="20.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -2052,7 +2101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="26" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -2066,7 +2115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="26" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -2080,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="26" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -2094,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="26" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -2108,7 +2157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="26" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -2122,7 +2171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="26" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -2136,7 +2185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="26" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -2150,7 +2199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="26" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2164,7 +2213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="26" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
@@ -2178,7 +2227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="26" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2192,7 +2241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="26" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
additions to the cell library
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="95">
   <si>
     <t>mouse name</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>Assess is poor.</t>
+  </si>
+  <si>
+    <t>CH_090414_C</t>
+  </si>
+  <si>
+    <t>Ra is poor for the later files.</t>
+  </si>
+  <si>
+    <t>CH_091114_F</t>
+  </si>
+  <si>
+    <t>Holding current is high</t>
   </si>
 </sst>
 </file>
@@ -1709,11 +1721,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2365,6 +2377,87 @@
         <v>89</v>
       </c>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="14">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="14">
+        <v>2</v>
+      </c>
+      <c r="C26" s="14">
+        <v>0</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="14">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
+      <c r="D27" s="14">
+        <v>1</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2381,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2477,6 +2570,88 @@
       </c>
       <c r="I3" s="17" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor change. some of the cell names were wrong (had the wrong date string attached to the names)
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="2"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="97">
   <si>
     <t>mouse name</t>
   </si>
@@ -281,15 +281,9 @@
     <t>A SOM+ cell without a PY cell to normalize by</t>
   </si>
   <si>
-    <t>CH_081411_C</t>
-  </si>
-  <si>
     <t>These data are kinda crummy (Vclamp issues on HS2)</t>
   </si>
   <si>
-    <t>CH_081411_D</t>
-  </si>
-  <si>
     <t>Access is poor on HS2</t>
   </si>
   <si>
@@ -312,6 +306,18 @@
   </si>
   <si>
     <t>Holding current is high</t>
+  </si>
+  <si>
+    <t>CH_081114_A</t>
+  </si>
+  <si>
+    <t>CH_081114_B</t>
+  </si>
+  <si>
+    <t>CH_081114_C</t>
+  </si>
+  <si>
+    <t>CH_081114_D</t>
   </si>
 </sst>
 </file>
@@ -1723,9 +1729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2142,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
@@ -2162,7 +2168,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -2188,7 +2194,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
@@ -2214,7 +2220,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B19" s="14">
         <v>2</v>
@@ -2240,7 +2246,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -2264,12 +2270,12 @@
         <v>9</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
@@ -2292,7 +2298,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
@@ -2316,12 +2322,12 @@
         <v>9</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="14">
         <v>1</v>
@@ -2345,12 +2351,12 @@
         <v>9</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
@@ -2374,12 +2380,12 @@
         <v>9</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -2405,7 +2411,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
@@ -2426,12 +2432,12 @@
         <v>9</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -2455,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2476,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2574,7 +2580,7 @@
     </row>
     <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
@@ -2600,7 +2606,7 @@
     </row>
     <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
@@ -2622,12 +2628,12 @@
         <v>9</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -2651,7 +2657,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some mice to the list. Also, i used the "sort" functionality and I'm hoping that this doesn't screw things up….
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Other_workbooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25480" windowHeight="16580" tabRatio="817" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="95">
   <si>
     <t>mouse name</t>
   </si>
@@ -266,13 +261,7 @@
     <t>IN?</t>
   </si>
   <si>
-    <t>CH_081411_A</t>
-  </si>
-  <si>
     <t>SOM</t>
-  </si>
-  <si>
-    <t>CH_081411_B</t>
   </si>
   <si>
     <t>This cell may need to be deleted due to space clamp</t>
@@ -394,7 +383,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -422,8 +411,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -474,8 +465,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -489,6 +483,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -502,6 +497,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -846,19 +842,19 @@
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.875" defaultRowHeight="26.1" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="75" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="33.875" style="1"/>
+    <col min="8" max="16384" width="33.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -878,7 +874,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="26" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -898,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="26" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -918,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="26" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -938,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="26" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -958,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="26" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -978,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="26" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -998,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="26" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -1021,7 +1017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="26" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1044,7 +1040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="26" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1067,7 +1063,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1090,7 +1086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="26" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1113,7 +1109,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="26" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="26" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="26" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="26" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="26" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1213,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="26" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="26" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1253,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="26" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="26" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="26" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1313,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="26" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1333,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="26" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1353,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="26" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1373,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="26" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1393,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="26" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1413,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="26" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="26" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1456,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="26" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1476,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="26" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1496,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="26" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="26" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1542,7 +1538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="26" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1562,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="26" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1585,7 +1581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="26" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="26" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="26" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1651,7 +1647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="26" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="26" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1691,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="26" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1729,25 +1725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="14.875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="14"/>
-    <col min="6" max="6" width="11.375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="14"/>
+    <col min="6" max="6" width="11.33203125" style="15" customWidth="1"/>
     <col min="7" max="7" width="13" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="15"/>
+    <col min="8" max="8" width="8.83203125" style="15"/>
     <col min="9" max="9" width="46.5" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="13"/>
+    <col min="10" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1776,9 +1772,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="21" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -1790,18 +1786,24 @@
         <v>1</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -1810,24 +1812,27 @@
         <v>1</v>
       </c>
       <c r="D3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="24.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B4" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="14">
         <v>1</v>
@@ -1836,24 +1841,21 @@
         <v>0</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -1862,30 +1864,30 @@
         <v>1</v>
       </c>
       <c r="D5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="H5" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="35.25" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B6" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
@@ -1893,9 +1895,6 @@
       <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>8</v>
-      </c>
       <c r="G6" s="15" t="s">
         <v>8</v>
       </c>
@@ -1903,157 +1902,154 @@
         <v>9</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
       </c>
       <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
         <v>0</v>
       </c>
-      <c r="D7" s="14">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="14">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="E8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
         <v>0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="14">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>54</v>
       </c>
       <c r="F9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="14">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="H10" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="14">
-        <v>1</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="14">
-        <v>1</v>
-      </c>
-      <c r="C12" s="14">
-        <v>1</v>
-      </c>
       <c r="D12" s="14">
         <v>1</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>8</v>
@@ -2062,18 +2058,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="31.5" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B13" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>12</v>
@@ -2081,68 +2077,68 @@
       <c r="F13" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="G13" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B14" s="14">
         <v>1</v>
       </c>
       <c r="C14" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="14">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
         <v>0</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="14">
-        <v>2</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>1</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="15" t="s">
+      <c r="F15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
@@ -2157,7 +2153,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>8</v>
@@ -2166,9 +2162,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -2186,15 +2182,15 @@
         <v>8</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
@@ -2215,12 +2211,12 @@
         <v>9</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B19" s="14">
         <v>2</v>
@@ -2235,18 +2231,18 @@
         <v>15</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -2261,7 +2257,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>8</v>
@@ -2270,12 +2266,12 @@
         <v>9</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
@@ -2296,9 +2292,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
@@ -2316,18 +2312,18 @@
         <v>8</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="14">
         <v>1</v>
@@ -2342,7 +2338,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>8</v>
@@ -2351,12 +2347,12 @@
         <v>9</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
@@ -2371,7 +2367,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>8</v>
@@ -2380,12 +2376,12 @@
         <v>9</v>
       </c>
       <c r="I24" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="13" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -2400,7 +2396,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>8</v>
@@ -2409,9 +2405,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
@@ -2432,12 +2428,12 @@
         <v>9</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -2461,15 +2457,15 @@
         <v>9</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I27">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="H17" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2480,23 +2476,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="8.875" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="18"/>
     <col min="9" max="9" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2525,12 +2522,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="13" customFormat="1">
       <c r="A2" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B2" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="14">
         <v>1</v>
@@ -2545,15 +2542,16 @@
         <v>8</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" s="13" customFormat="1">
       <c r="A3" s="13" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2562,25 +2560,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" s="13" customFormat="1">
       <c r="A4" s="13" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
@@ -2592,27 +2590,28 @@
         <v>1</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1">
       <c r="A5" s="13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="14">
         <v>1</v>
@@ -2620,20 +2619,19 @@
       <c r="E5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="15" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1">
       <c r="A6" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -2642,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>15</v>
@@ -2650,21 +2648,161 @@
       <c r="F6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>92</v>
+      <c r="I6" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1">
+      <c r="A11" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I9">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="H2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2676,14 +2814,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.375" defaultRowHeight="26.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="20.375" style="6"/>
-    <col min="4" max="4" width="20.375" style="7"/>
-    <col min="5" max="16384" width="20.375" style="6"/>
+    <col min="1" max="3" width="20.33203125" style="6"/>
+    <col min="4" max="4" width="20.33203125" style="7"/>
+    <col min="5" max="16384" width="20.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -2697,7 +2835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="26" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -2711,7 +2849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="26" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -2725,7 +2863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="26" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -2739,7 +2877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="26" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -2753,7 +2891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="26" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -2767,7 +2905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="26" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -2781,7 +2919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="26" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -2795,7 +2933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="26" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2809,7 +2947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="26" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
@@ -2823,7 +2961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="26" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2837,7 +2975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="26" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
changes to the population cell list
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Other_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Other_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="114">
   <si>
     <t>mouse name</t>
   </si>
@@ -354,6 +354,21 @@
   </si>
   <si>
     <t>AK_101314_A</t>
+  </si>
+  <si>
+    <t>layer cell 2</t>
+  </si>
+  <si>
+    <t>layer cell 1</t>
+  </si>
+  <si>
+    <t>Need to confirm cell type.</t>
+  </si>
+  <si>
+    <t>Need to confirm cell type. And brain region</t>
+  </si>
+  <si>
+    <t>AK_101314_C</t>
   </si>
 </sst>
 </file>
@@ -1785,11 +1800,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1800,12 +1815,13 @@
     <col min="5" max="5" width="8.875" style="14"/>
     <col min="6" max="6" width="11.375" style="15" customWidth="1"/>
     <col min="7" max="7" width="13" style="15" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="15"/>
-    <col min="9" max="9" width="46.5" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="13"/>
+    <col min="8" max="8" width="9.5" style="15" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="15" customWidth="1"/>
+    <col min="10" max="10" width="46.5" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1828,13 +1844,16 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>68</v>
       </c>
@@ -1859,11 +1878,14 @@
       <c r="H2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>70</v>
       </c>
@@ -1888,8 +1910,11 @@
       <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>70</v>
       </c>
@@ -1911,11 +1936,14 @@
       <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>73</v>
       </c>
@@ -1937,11 +1965,14 @@
       <c r="H5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>73</v>
       </c>
@@ -1963,11 +1994,14 @@
       <c r="H6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>49</v>
       </c>
@@ -1986,11 +2020,14 @@
       <c r="H7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
@@ -2009,11 +2046,14 @@
       <c r="H8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>56</v>
       </c>
@@ -2038,11 +2078,14 @@
       <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>58</v>
       </c>
@@ -2067,8 +2110,11 @@
       <c r="H10" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>60</v>
       </c>
@@ -2093,11 +2139,14 @@
       <c r="H11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>62</v>
       </c>
@@ -2119,8 +2168,11 @@
       <c r="H12" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>64</v>
       </c>
@@ -2145,8 +2197,11 @@
       <c r="H13" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>65</v>
       </c>
@@ -2171,11 +2226,14 @@
       <c r="H14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>67</v>
       </c>
@@ -2197,8 +2255,11 @@
       <c r="H15" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>91</v>
       </c>
@@ -2223,8 +2284,11 @@
       <c r="H16" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>91</v>
       </c>
@@ -2249,8 +2313,11 @@
       <c r="H17" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>92</v>
       </c>
@@ -2272,11 +2339,14 @@
       <c r="H18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>92</v>
       </c>
@@ -2298,11 +2368,14 @@
       <c r="H19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>93</v>
       </c>
@@ -2324,11 +2397,14 @@
       <c r="H20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>94</v>
       </c>
@@ -2350,8 +2426,11 @@
       <c r="H21" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>94</v>
       </c>
@@ -2376,11 +2455,14 @@
       <c r="H22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>84</v>
       </c>
@@ -2405,11 +2487,14 @@
       <c r="H23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>84</v>
       </c>
@@ -2434,11 +2519,14 @@
       <c r="H24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>87</v>
       </c>
@@ -2463,8 +2551,11 @@
       <c r="H25" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>87</v>
       </c>
@@ -2486,11 +2577,14 @@
       <c r="H26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>89</v>
       </c>
@@ -2515,11 +2609,14 @@
       <c r="H27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>95</v>
       </c>
@@ -2541,11 +2638,14 @@
       <c r="H28" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>95</v>
       </c>
@@ -2567,11 +2667,14 @@
       <c r="H29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>97</v>
       </c>
@@ -2593,11 +2696,14 @@
       <c r="H30" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>97</v>
       </c>
@@ -2619,11 +2725,14 @@
       <c r="H31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>98</v>
       </c>
@@ -2645,11 +2754,14 @@
       <c r="H32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>98</v>
       </c>
@@ -2671,11 +2783,14 @@
       <c r="H33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I33" s="19" t="s">
+      <c r="I33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>100</v>
       </c>
@@ -2697,11 +2812,14 @@
       <c r="H34" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>100</v>
       </c>
@@ -2723,11 +2841,14 @@
       <c r="H35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="19" t="s">
+      <c r="I35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>102</v>
       </c>
@@ -2749,11 +2870,14 @@
       <c r="H36" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I36" s="19" t="s">
+      <c r="I36" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J36" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>104</v>
       </c>
@@ -2775,11 +2899,14 @@
       <c r="H37" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="I37" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>104</v>
       </c>
@@ -2801,8 +2928,43 @@
       <c r="H38" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="I38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J38" s="13" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="14">
+        <v>1</v>
+      </c>
+      <c r="C39" s="14">
+        <v>1</v>
+      </c>
+      <c r="D39" s="14">
+        <v>1</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2821,11 +2983,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2835,11 +2997,11 @@
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="10.375" customWidth="1"/>
     <col min="6" max="6" width="8.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="18"/>
-    <col min="9" max="9" width="46.5" customWidth="1"/>
+    <col min="9" max="9" width="10.25" style="18" customWidth="1"/>
+    <col min="10" max="10" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2862,13 +3024,16 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>70</v>
       </c>
@@ -2893,9 +3058,12 @@
       <c r="H2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
@@ -2920,9 +3088,12 @@
       <c r="H3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -2947,9 +3118,12 @@
       <c r="H4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>91</v>
       </c>
@@ -2974,8 +3148,11 @@
       <c r="H5" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>92</v>
       </c>
@@ -2998,11 +3175,14 @@
       <c r="H6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>87</v>
       </c>
@@ -3027,9 +3207,12 @@
       <c r="H7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>87</v>
       </c>
@@ -3052,11 +3235,14 @@
       <c r="H8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>89</v>
       </c>
@@ -3081,11 +3267,14 @@
       <c r="H9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
@@ -3110,8 +3299,11 @@
       <c r="H10" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>73</v>
       </c>
@@ -3134,11 +3326,14 @@
       <c r="H11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>95</v>
       </c>
@@ -3161,11 +3356,14 @@
       <c r="H12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>95</v>
       </c>
@@ -3188,11 +3386,14 @@
       <c r="H13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>97</v>
       </c>
@@ -3215,11 +3416,14 @@
       <c r="H14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>97</v>
       </c>
@@ -3241,11 +3445,14 @@
       <c r="H15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>98</v>
       </c>
@@ -3267,11 +3474,14 @@
       <c r="H16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>98</v>
       </c>
@@ -3293,11 +3503,14 @@
       <c r="H17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>100</v>
       </c>
@@ -3319,11 +3532,14 @@
       <c r="H18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>100</v>
       </c>
@@ -3346,11 +3562,14 @@
       <c r="H19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>102</v>
       </c>
@@ -3372,11 +3591,14 @@
       <c r="H20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>104</v>
       </c>
@@ -3399,11 +3621,14 @@
       <c r="H21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>104</v>
       </c>
@@ -3426,11 +3651,14 @@
       <c r="H22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>108</v>
       </c>
@@ -3452,11 +3680,14 @@
       <c r="H23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="19" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>108</v>
       </c>
@@ -3478,8 +3709,43 @@
       <c r="H24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="19" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="14">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed a few laminar positions
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Other_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Other_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="121">
   <si>
     <t>mouse name</t>
   </si>
@@ -330,9 +330,6 @@
   </si>
   <si>
     <t>AK_092914_D</t>
-  </si>
-  <si>
-    <t>Need to check HVA location and cell type and layer</t>
   </si>
   <si>
     <t>CH_100614_B</t>
@@ -1829,9 +1826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1871,10 +1868,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -2206,11 +2203,8 @@
       <c r="G13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>9</v>
-      </c>
       <c r="I13" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2514,10 +2508,10 @@
         <v>8</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="J24" s="13" t="s">
         <v>85</v>
@@ -2789,10 +2783,10 @@
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2823,7 +2817,7 @@
     </row>
     <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -2845,12 +2839,12 @@
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" s="14">
         <v>2</v>
@@ -2871,12 +2865,12 @@
         <v>9</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B38" s="14">
         <v>3</v>
@@ -2897,12 +2891,12 @@
         <v>44</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="14">
         <v>1</v>
@@ -2929,12 +2923,12 @@
         <v>9</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="14">
         <v>1</v>
@@ -2963,7 +2957,7 @@
     </row>
     <row r="41" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B41" s="14">
         <v>1</v>
@@ -2988,7 +2982,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" s="14">
         <v>1</v>
@@ -3009,12 +3003,12 @@
         <v>9</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="14">
         <v>1</v>
@@ -3037,7 +3031,7 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3058,9 +3052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3098,10 +3092,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -3572,10 +3566,10 @@
         <v>8</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3608,33 +3602,33 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="14">
+        <v>1</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="B20" s="14">
-        <v>1</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="14">
-        <v>0</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="14">
         <v>2</v>
@@ -3657,12 +3651,12 @@
         <v>9</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="14">
         <v>3</v>
@@ -3685,12 +3679,12 @@
         <v>44</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="14">
         <v>1</v>
@@ -3711,12 +3705,12 @@
         <v>9</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
@@ -3737,12 +3731,12 @@
         <v>9</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -3769,12 +3763,12 @@
         <v>9</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26" s="14">
         <v>1</v>
@@ -3803,7 +3797,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="14">
         <v>2</v>
@@ -3824,12 +3818,12 @@
         <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
@@ -3852,7 +3846,7 @@
     </row>
     <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="14">
         <v>1</v>
@@ -3875,33 +3869,33 @@
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="14">
+        <v>1</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" t="s">
         <v>118</v>
-      </c>
-      <c r="B30" s="14">
-        <v>1</v>
-      </c>
-      <c r="C30" s="14">
-        <v>0</v>
-      </c>
-      <c r="D30" s="14">
-        <v>1</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking HVA location against the histology. A few modifications, and I deleted AK_092914_C cell 2 from the NMDAR list due to inconsistencies in data collection.
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="114">
   <si>
     <t>mouse name</t>
   </si>
@@ -284,24 +284,15 @@
     <t>CH_090414_A</t>
   </si>
   <si>
-    <t>Different Vhold for HS1/2 for Erev excitation</t>
-  </si>
-  <si>
     <t>Assess is poor.</t>
   </si>
   <si>
     <t>CH_090414_C</t>
   </si>
   <si>
-    <t>Ra is poor for the later files.</t>
-  </si>
-  <si>
     <t>CH_091114_F</t>
   </si>
   <si>
-    <t>Holding current is high</t>
-  </si>
-  <si>
     <t>CH_081114_A</t>
   </si>
   <si>
@@ -317,30 +308,18 @@
     <t>AK_092914_A</t>
   </si>
   <si>
-    <t>Need to check HVA location</t>
-  </si>
-  <si>
     <t>AK_092914_B</t>
   </si>
   <si>
     <t>AK_092914_C</t>
   </si>
   <si>
-    <t>Need to check HVA location and cell type</t>
-  </si>
-  <si>
     <t>AK_092914_D</t>
   </si>
   <si>
-    <t>Need to check HVA location and cell type and layer</t>
-  </si>
-  <si>
     <t>CH_100614_B</t>
   </si>
   <si>
-    <t>Vhold -20 seems like it has Ca2+ contamination</t>
-  </si>
-  <si>
     <t>CH_100614_C</t>
   </si>
   <si>
@@ -368,9 +347,6 @@
     <t>Not 100% sure on cell type</t>
   </si>
   <si>
-    <t>Confirm brain region</t>
-  </si>
-  <si>
     <t>CH_141020_A</t>
   </si>
   <si>
@@ -392,14 +368,14 @@
     <t>confirm brain region and cell type</t>
   </si>
   <si>
-    <t>need to confirm region and cell type</t>
+    <t>originally this was AL, but I think it's UND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,6 +423,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -506,7 +488,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -572,6 +554,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -942,7 +929,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1829,9 +1816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1871,10 +1858,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -2270,7 +2257,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
@@ -2299,7 +2286,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -2328,7 +2315,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
@@ -2354,7 +2341,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B19" s="14">
         <v>2</v>
@@ -2380,7 +2367,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -2406,7 +2393,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
@@ -2429,7 +2416,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
@@ -2488,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2519,13 +2506,10 @@
       <c r="I24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -2554,7 +2538,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
@@ -2574,13 +2558,10 @@
       <c r="I26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -2606,13 +2587,10 @@
       <c r="I27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="13" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
@@ -2632,13 +2610,11 @@
       <c r="I28" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B29" s="14">
         <v>2</v>
@@ -2650,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>8</v>
@@ -2658,13 +2634,11 @@
       <c r="I29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B30" s="14">
         <v>2</v>
@@ -2676,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>8</v>
@@ -2685,13 +2659,13 @@
       <c r="I30" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J30" s="19" t="s">
-        <v>96</v>
+      <c r="J30" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B31" s="14">
         <v>1</v>
@@ -2711,13 +2685,11 @@
       <c r="I31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J31" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B32" s="14">
         <v>1</v>
@@ -2729,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>54</v>
@@ -2737,13 +2709,11 @@
       <c r="I32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B33" s="14">
         <v>3</v>
@@ -2764,13 +2734,11 @@
       <c r="I33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J33" s="19" t="s">
-        <v>99</v>
-      </c>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B34" s="14">
         <v>4</v>
@@ -2789,15 +2757,13 @@
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>101</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B35" s="14">
         <v>5</v>
@@ -2817,13 +2783,11 @@
       <c r="I35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J35" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -2844,13 +2808,11 @@
         <v>9</v>
       </c>
       <c r="I36" s="18"/>
-      <c r="J36" s="19" t="s">
-        <v>103</v>
-      </c>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B37" s="14">
         <v>2</v>
@@ -2871,12 +2833,12 @@
         <v>9</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B38" s="14">
         <v>3</v>
@@ -2897,12 +2859,12 @@
         <v>44</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B39" s="14">
         <v>1</v>
@@ -2928,13 +2890,10 @@
       <c r="I39" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="13" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B40" s="14">
         <v>1</v>
@@ -2963,7 +2922,7 @@
     </row>
     <row r="41" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B41" s="14">
         <v>1</v>
@@ -2988,7 +2947,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B42" s="14">
         <v>1</v>
@@ -3008,13 +2967,13 @@
       <c r="H42" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J42" s="13" t="s">
-        <v>117</v>
+      <c r="J42" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B43" s="14">
         <v>1</v>
@@ -3037,7 +2996,7 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3004,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3056,11 +3015,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3098,10 +3057,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -3199,7 +3158,7 @@
     </row>
     <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
@@ -3228,7 +3187,7 @@
     </row>
     <row r="6" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -3256,7 +3215,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
@@ -3286,7 +3245,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -3312,7 +3271,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="14">
         <v>1</v>
@@ -3368,6 +3327,7 @@
       <c r="I10" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -3393,10 +3353,11 @@
         <v>9</v>
       </c>
       <c r="I11" s="15"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" s="14">
         <v>1</v>
@@ -3418,13 +3379,11 @@
       <c r="I12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" s="14">
         <v>2</v>
@@ -3436,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="15" t="s">
@@ -3446,13 +3405,11 @@
       <c r="I13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B14" s="14">
         <v>1</v>
@@ -3478,7 +3435,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
@@ -3490,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>8</v>
@@ -3502,10 +3459,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B16" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="14">
         <v>0</v>
@@ -3514,24 +3471,22 @@
         <v>1</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="19" t="s">
-        <v>96</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B17" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="14">
         <v>0</v>
@@ -3546,18 +3501,16 @@
         <v>8</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" s="14">
         <v>0</v>
@@ -3566,78 +3519,76 @@
         <v>1</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>15</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F18" s="21"/>
       <c r="G18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="15"/>
+      <c r="I18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B19" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B20" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>103</v>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B21" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="14">
         <v>0</v>
@@ -3646,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15" t="s">
@@ -3654,95 +3605,96 @@
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="J21" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="14">
+        <v>1</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="19" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="14">
-        <v>3</v>
-      </c>
-      <c r="C22" s="14">
-        <v>0</v>
-      </c>
-      <c r="D22" s="14">
-        <v>1</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B23" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="18" t="s">
+      <c r="G23" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B24" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -3754,59 +3706,53 @@
         <v>1</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>113</v>
+      <c r="H25" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B26" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>9</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B27" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="14">
         <v>0</v>
@@ -3815,93 +3761,67 @@
         <v>1</v>
       </c>
       <c r="E27" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="14">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0</v>
+      </c>
+      <c r="E28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="14">
-        <v>1</v>
-      </c>
-      <c r="C28" s="14">
-        <v>0</v>
-      </c>
-      <c r="D28" s="14">
-        <v>1</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="15"/>
+      <c r="J28" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B29" s="14">
         <v>1</v>
       </c>
       <c r="C29" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="14">
-        <v>1</v>
-      </c>
-      <c r="C30" s="14">
-        <v>0</v>
-      </c>
-      <c r="D30" s="14">
-        <v>1</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" t="s">
-        <v>119</v>
+        <v>7</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to clean up after a sloppy conflict resolution
</commit_message>
<xml_diff>
--- a/Other_workbooks/Cell_Library.xlsx
+++ b/Other_workbooks/Cell_Library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="2"/>
+    <workbookView xWindow="1260" yWindow="900" windowWidth="25485" windowHeight="16575" tabRatio="817" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V1_AxonStim" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="113">
   <si>
     <t>mouse name</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>analyze cell 1</t>
-  </si>
-  <si>
-    <t>IN?</t>
   </si>
   <si>
     <t>SOM</t>
@@ -1816,9 +1813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1858,10 +1855,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -2072,10 +2069,10 @@
         <v>54</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>9</v>
@@ -2193,11 +2190,8 @@
       <c r="G13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>9</v>
-      </c>
       <c r="I13" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2257,7 +2251,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
@@ -2272,7 +2266,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>8</v>
@@ -2286,7 +2280,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -2304,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H17" s="15" t="s">
         <v>44</v>
@@ -2315,7 +2309,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
@@ -2336,12 +2330,12 @@
         <v>9</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="14">
         <v>2</v>
@@ -2356,18 +2350,18 @@
         <v>15</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>9</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -2388,12 +2382,12 @@
         <v>9</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
@@ -2416,7 +2410,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
@@ -2434,7 +2428,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="15" t="s">
         <v>9</v>
@@ -2443,12 +2437,12 @@
         <v>9</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="14">
         <v>1</v>
@@ -2463,7 +2457,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>8</v>
@@ -2475,12 +2469,12 @@
         <v>9</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
@@ -2495,21 +2489,21 @@
         <v>15</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -2524,7 +2518,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>8</v>
@@ -2538,7 +2532,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
@@ -2561,7 +2555,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -2590,7 +2584,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
@@ -2614,7 +2608,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="14">
         <v>2</v>
@@ -2638,7 +2632,7 @@
     </row>
     <row r="30" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="14">
         <v>2</v>
@@ -2660,12 +2654,12 @@
         <v>9</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" s="14">
         <v>1</v>
@@ -2689,7 +2683,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" s="14">
         <v>1</v>
@@ -2713,7 +2707,7 @@
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="14">
         <v>3</v>
@@ -2738,7 +2732,7 @@
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="14">
         <v>4</v>
@@ -2763,7 +2757,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="14">
         <v>5</v>
@@ -2787,7 +2781,7 @@
     </row>
     <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -2812,7 +2806,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="14">
         <v>2</v>
@@ -2833,12 +2827,12 @@
         <v>9</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="14">
         <v>3</v>
@@ -2859,12 +2853,12 @@
         <v>44</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B39" s="14">
         <v>1</v>
@@ -2893,7 +2887,7 @@
     </row>
     <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" s="14">
         <v>1</v>
@@ -2922,7 +2916,7 @@
     </row>
     <row r="41" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" s="14">
         <v>1</v>
@@ -2947,7 +2941,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="14">
         <v>1</v>
@@ -2968,12 +2962,12 @@
         <v>9</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="14">
         <v>1</v>
@@ -2996,7 +2990,7 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3017,9 +3011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3057,10 +3051,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>50</v>
@@ -3158,7 +3152,7 @@
     </row>
     <row r="5" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
@@ -3176,7 +3170,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>44</v>
@@ -3187,7 +3181,7 @@
     </row>
     <row r="6" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -3210,12 +3204,12 @@
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
@@ -3230,7 +3224,7 @@
         <v>54</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>8</v>
@@ -3245,7 +3239,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="14">
         <v>2</v>
@@ -3271,7 +3265,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="14">
         <v>1</v>
@@ -3357,7 +3351,7 @@
     </row>
     <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="14">
         <v>1</v>
@@ -3383,7 +3377,7 @@
     </row>
     <row r="13" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="14">
         <v>2</v>
@@ -3409,7 +3403,7 @@
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="14">
         <v>1</v>
@@ -3435,7 +3429,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
@@ -3459,7 +3453,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="14">
         <v>3</v>
@@ -3483,7 +3477,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="14">
         <v>4</v>
@@ -3507,7 +3501,7 @@
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="14">
         <v>5</v>
@@ -3533,7 +3527,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="14">
         <v>1</v>
@@ -3557,7 +3551,7 @@
     </row>
     <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -3580,12 +3574,12 @@
         <v>9</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="14">
         <v>3</v>
@@ -3608,12 +3602,12 @@
         <v>44</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="14">
         <v>1</v>
@@ -3634,12 +3628,12 @@
         <v>9</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="14">
         <v>2</v>
@@ -3660,12 +3654,12 @@
         <v>9</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="14">
         <v>1</v>
@@ -3694,7 +3688,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -3723,7 +3717,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
@@ -3744,12 +3738,12 @@
         <v>9</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -3772,7 +3766,7 @@
     </row>
     <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
@@ -3795,33 +3789,33 @@
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="14">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14">
+        <v>0</v>
+      </c>
+      <c r="D29" s="14">
+        <v>1</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="25" t="s">
         <v>110</v>
-      </c>
-      <c r="B29" s="14">
-        <v>1</v>
-      </c>
-      <c r="C29" s="14">
-        <v>0</v>
-      </c>
-      <c r="D29" s="14">
-        <v>1</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="25" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>